<commit_message>
Check almost fully functional. Only issue is that I forgot other pieces can stop a check lol, so I limited it to the king
</commit_message>
<xml_diff>
--- a/Functional Testing Checklist.xlsx
+++ b/Functional Testing Checklist.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B62002E-DDB8-41BA-8570-52A76876A0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Functional Testing Checklist</t>
   </si>
@@ -73,12 +74,24 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>Lethiwe Mwendwa</t>
+  </si>
+  <si>
+    <t>N1103546</t>
+  </si>
+  <si>
+    <t>Amin Safaei</t>
+  </si>
+  <si>
+    <t>CSI3 (I think…?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,28 +178,28 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -217,13 +230,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1466850</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>171467</xdr:rowOff>
+      <xdr:colOff>2743200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>189593</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="What is a Functional Requirement? Specification, Types, EXAMPLES"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="What is a Functional Requirement? Specification, Types, EXAMPLES">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -244,7 +263,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="1828800" y="3933826"/>
-          <a:ext cx="2924175" cy="914416"/>
+          <a:ext cx="4200525" cy="1313542"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -528,11 +547,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,129 +562,137 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="3" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="6"/>
     </row>
     <row r="8" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
@@ -674,11 +701,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="D14:F14"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D5:E5"/>
@@ -689,6 +711,11 @@
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="D13:F13"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="D14:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>